<commit_message>
Atualização Casos de uso 11~19
</commit_message>
<xml_diff>
--- a/Arquivo/Casos de Uso/Casos de uso - Quadro(cenario).xlsx
+++ b/Arquivo/Casos de Uso/Casos de uso - Quadro(cenario).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\_\Fatec\ADS\ES2 - Engenharia de Software II\Github\ES2N_Capivara_Empacada\Arquivo\Casos de Uso\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\FATEC 2020\5 Semestre\Engenharia de Software 2\Projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6918205-DDCD-46F7-AEA6-1E5FD5A59185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D15F6B2F-57CF-4EA1-B63D-8D5CBEAFE2EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="945" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="28800" windowHeight="11385" tabRatio="945" firstSheet="15" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RF01 - Fazer Login" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="195">
   <si>
     <t>Caso de Uso</t>
   </si>
@@ -198,12 +198,6 @@
     <t>O veterinário deve receber um sms ou e-mail</t>
   </si>
   <si>
-    <t>1. O sistema busca os dados de todos os animais cadastrados
-2. O sistema verifica se algum dos pets possui anormalidades em seus registros
-3. O sistema registra todas as anormalidades detectadas
-4. O sistema envia uma notificação do tipo selecionado pelo usuário para o veterinário responsável pelo pet</t>
-  </si>
-  <si>
     <t>Gerenciar Estoque de ração</t>
   </si>
   <si>
@@ -245,36 +239,12 @@
 2. Dosador deve possuir carga de energia ou estar conectado à tomada.</t>
   </si>
   <si>
-    <t>1. Dosador calcula o peso atual do pote da ração
-2. Dosador atualiza os dados de quantidade de ração</t>
-  </si>
-  <si>
     <t>Notificar usuário</t>
   </si>
   <si>
     <t>1. Usuário deve possuir cadastro
 2. Usuário deve possuir ao menos um equipamento cadastrado
 3. Usário deve habilitar o envio de e-mail</t>
-  </si>
-  <si>
-    <t>1. Sistema consulta no banco dados para envio de avisos
-2. Sistema envia notificação para o usuário</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. O usuário acessa o aplicativo
-2. O usuário seleciona a opção de cadastrar nova conta
-3. O usuário preenche os dados requeridos (Nome de usuário, E-mail e senha)
-4. O usuário seleciona a opção para cadastrar
-</t>
-  </si>
-  <si>
-    <t>5. O sistema registra o cadastro no banco de dados
-6. O sistema realiza o login no aplicativo</t>
-  </si>
-  <si>
-    <t>1. O usuário acessa o aplicativo
-2. O usuário realiza o login
-3. O usuário acessa a tela de gerenciamento da conta</t>
   </si>
   <si>
     <t>4. O sistema exibe as informações cadastradas para o usuário atual</t>
@@ -289,32 +259,11 @@
     <t>7. O usuário realiza a confirmação</t>
   </si>
   <si>
-    <t>8. O sistema realiza as alterações no banco de dados
-9. O sistema exibe a tela inicial</t>
-  </si>
-  <si>
-    <t>5. O usuário realiza as alterações nos campos desejados
-6. O usuário seleciona a opção para salvar as alterações realizadas</t>
-  </si>
-  <si>
-    <t>7. O sistema salva as alterações
-8. O sistema exibe a tela principal</t>
-  </si>
-  <si>
     <t>1. O usuário acessa a tela principal do aplicativo
 2. O usuário acessa a tela de gerenciamento veterinários</t>
   </si>
   <si>
     <t>3. O sistema lista todos os veterinários já cadastrados para esse usuário</t>
-  </si>
-  <si>
-    <t>4. O usuário seleciona a opção de cadastrar novo veterinário
-5. O usuário preenche os campos (Nome, Bairro, Logradouro, Número, Telefone, E-mail e preferência para notificação)
-6. O usuário o usuário seleciona a opção para salvar o novo veterinário</t>
-  </si>
-  <si>
-    <t>7. O sistema registra a alteração
-8. O sistema recarrega a lista de veterinários atualizada</t>
   </si>
   <si>
     <t>4. O usuário seleciona um dos veterinários listados</t>
@@ -332,10 +281,6 @@
     <t>8. O usuário confirma a exclusão</t>
   </si>
   <si>
-    <t>9. O sistema registra a alteração
-10. O sistema recarrega a lista de veterinários atualizada</t>
-  </si>
-  <si>
     <t>6. O usuário seleciona a opção de alteração</t>
   </si>
   <si>
@@ -346,35 +291,13 @@
 9. O usuário seleciona a opção para salvar as alterações</t>
   </si>
   <si>
-    <t>10. O sistema registra a alteração
-11. O sistema recarrega a lista de veterinários atualizada</t>
-  </si>
-  <si>
-    <t>1. O usuário acessa a tela principal do aplicativo
-2. O usuário acessa a tela de gerenciamento de estoque</t>
-  </si>
-  <si>
     <t>3. O sistema exibe a quantidade de ração atualmente em seu estoque</t>
   </si>
   <si>
     <t>4. O usuário altera a quantidade atual</t>
   </si>
   <si>
-    <t>5. O sistema grava sua alteração
-6. O sistema exibe a nova quantidade na tela</t>
-  </si>
-  <si>
-    <t>1. O usuário acessa a tela principal do aplicativo
-2. O usuário acessa a tela de gerenciamento de notificações</t>
-  </si>
-  <si>
     <t>3. O sistema exibe as notificações habilitadas</t>
-  </si>
-  <si>
-    <t>1. O usuário acessa a tela principal do aplicativo
-2. O usuário acessa a tela de gerenciamento de notificações
-3. O usuário habilita ou desabilita os tipos de notificação que deseja receber
-4. O usuário clica em "Salvar" para armazenar as informações no servidor</t>
   </si>
   <si>
     <t>5. O sistema confirma a atualização das configurações</t>
@@ -383,17 +306,7 @@
     <t>2.1.2 Sistema apresenta os equipamentos cadastrados para o usuário</t>
   </si>
   <si>
-    <t>2.2. Selecionada a opção Autorizar Comunicação
-2.2.1 Usuário confirma os dados do equipamento</t>
-  </si>
-  <si>
     <t>2.2.3 Sistema permite o comunicação entre os equipamentos</t>
-  </si>
-  <si>
-    <t>1. Usuário acessa a tela de cadastros de PETs
-2. Usuário seleciona a opção consultar comunicação
-2.1. Seleciona o equipamento
-2.1.1 Seleciona o assistente inteligente</t>
   </si>
   <si>
     <t>1. O usuário acessa o APP</t>
@@ -591,6 +504,147 @@
   <si>
     <t>9. Sistema permite a exclusão do equipamento</t>
   </si>
+  <si>
+    <t>1. O usuário acessa o aplicativo</t>
+  </si>
+  <si>
+    <t>2. O usuário realiza o login</t>
+  </si>
+  <si>
+    <t>3. O usuário acessa a tela de gerenciamento da conta</t>
+  </si>
+  <si>
+    <t>2. O usuário seleciona a opção de cadastrar nova conta</t>
+  </si>
+  <si>
+    <t>3. O usuário preenche os dados requeridos (Nome de usuário, E-mail e senha)</t>
+  </si>
+  <si>
+    <t>4. O usuário seleciona a opção para cadastrar</t>
+  </si>
+  <si>
+    <t>5. O sistema registra o cadastro no banco de dados</t>
+  </si>
+  <si>
+    <t>6. O sistema realiza o login no aplicativo</t>
+  </si>
+  <si>
+    <t>8. O sistema realiza as alterações no banco de dados</t>
+  </si>
+  <si>
+    <t>9. O sistema exibe a tela inicial</t>
+  </si>
+  <si>
+    <t>5. O usuário realiza as alterações nos campos desejados</t>
+  </si>
+  <si>
+    <t>6. O usuário seleciona a opção para salvar as alterações realizadas</t>
+  </si>
+  <si>
+    <t>7. O sistema salva as alterações</t>
+  </si>
+  <si>
+    <t>8. O sistema exibe a tela principal</t>
+  </si>
+  <si>
+    <t>1. O usuário acessa a tela principal do aplicativo</t>
+  </si>
+  <si>
+    <t>2. O usuário acessa a tela de gerenciamento veterinários</t>
+  </si>
+  <si>
+    <t>4. O usuário seleciona a opção de cadastrar novo veterinário</t>
+  </si>
+  <si>
+    <t>5. O usuário preenche os campos (Nome, Bairro, Logradouro, Número, Telefone, E-mail e preferência para notificação)</t>
+  </si>
+  <si>
+    <t>6. O usuário o usuário seleciona a opção para salvar o novo veterinário</t>
+  </si>
+  <si>
+    <t>7. O sistema registra a alteração</t>
+  </si>
+  <si>
+    <t>8. O sistema recarrega a lista de veterinários atualizada</t>
+  </si>
+  <si>
+    <t>2. O usuário acessa a tela de gerenciamento veterinário</t>
+  </si>
+  <si>
+    <t>9. O sistema registra a alteração</t>
+  </si>
+  <si>
+    <t>10. O sistema recarrega a lista de veterinários atualizada</t>
+  </si>
+  <si>
+    <t>8. O usuário altera os campos desejados</t>
+  </si>
+  <si>
+    <t>9. O usuário seleciona a opção para salvar as alterações</t>
+  </si>
+  <si>
+    <t>11. O sistema recarrega a lista de veterinários atualizada</t>
+  </si>
+  <si>
+    <t>10. O sistema registra a alteração</t>
+  </si>
+  <si>
+    <t>1. O sistema busca os dados de todos os animais cadastrados</t>
+  </si>
+  <si>
+    <t>2. O sistema verifica se algum dos pets possui anormalidades em seus registros</t>
+  </si>
+  <si>
+    <t>3. O sistema registra todas as anormalidades detectadas</t>
+  </si>
+  <si>
+    <t>4. O sistema envia uma notificação do tipo selecionado pelo usuário para o veterinário responsável pelo pet</t>
+  </si>
+  <si>
+    <t>2. O usuário acessa a tela de gerenciamento de estoque</t>
+  </si>
+  <si>
+    <t>5. O sistema grava sua alteração</t>
+  </si>
+  <si>
+    <t>6. O sistema exibe a nova quantidade na tela</t>
+  </si>
+  <si>
+    <t>2. O usuário acessa a tela de gerenciamento de notificações</t>
+  </si>
+  <si>
+    <t>3. O usuário habilita ou desabilita os tipos de notificação que deseja receber</t>
+  </si>
+  <si>
+    <t>4. O usuário clica em "Salvar" para armazenar as informações no servidor</t>
+  </si>
+  <si>
+    <t>2. Usuário seleciona a opção consultar comunicação</t>
+  </si>
+  <si>
+    <t>2.1. Seleciona o equipamento</t>
+  </si>
+  <si>
+    <t>2.1.1 Seleciona o assistente inteligente</t>
+  </si>
+  <si>
+    <t>2.2. Selecionada a opção Autorizar Comunicação</t>
+  </si>
+  <si>
+    <t>2.2.1 Usuário confirma os dados do equipamento</t>
+  </si>
+  <si>
+    <t>1. Dosador calcula o peso atual do pote da ração</t>
+  </si>
+  <si>
+    <t>2. Dosador atualiza os dados de quantidade de ração</t>
+  </si>
+  <si>
+    <t>1. Sistema consulta no banco dados para envio de avisos</t>
+  </si>
+  <si>
+    <t>2. Sistema envia notificação para o usuário</t>
+  </si>
 </sst>
 </file>
 
@@ -621,15 +675,13 @@
       <charset val="1"/>
     </font>
     <font>
-      <u/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -661,7 +713,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -708,11 +760,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -755,7 +820,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -782,16 +846,59 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1235,39 +1342,39 @@
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="19" t="s">
-        <v>102</v>
+      <c r="A7" s="18" t="s">
+        <v>83</v>
       </c>
-      <c r="B7" s="19"/>
+      <c r="B7" s="18"/>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="19" t="s">
-        <v>103</v>
+      <c r="A8" s="18" t="s">
+        <v>84</v>
       </c>
-      <c r="B8" s="19"/>
+      <c r="B8" s="18"/>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="19"/>
-      <c r="B9" s="19" t="s">
-        <v>104</v>
+      <c r="A9" s="18"/>
+      <c r="B9" s="18" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="B10" s="3"/>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="15"/>
       <c r="B11" s="3" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="4"/>
       <c r="B12" s="2" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -5260,7 +5367,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:E1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B14" sqref="A1:B14"/>
     </sheetView>
   </sheetViews>
@@ -5316,21 +5423,21 @@
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
     </row>
     <row r="7" spans="1:5" ht="25.5">
       <c r="A7" s="15" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="B7" s="3"/>
       <c r="D7" s="7"/>
-      <c r="E7" s="21"/>
+      <c r="E7" s="20"/>
     </row>
     <row r="8" spans="1:5" ht="51">
       <c r="A8" s="4"/>
       <c r="B8" s="15" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
@@ -5338,14 +5445,14 @@
     <row r="9" spans="1:5" ht="25.5">
       <c r="A9" s="4"/>
       <c r="B9" s="15" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="4" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
       <c r="B10" s="15"/>
       <c r="D10" s="7"/>
@@ -5353,7 +5460,7 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="4" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
       <c r="B11" s="15"/>
       <c r="D11" s="7"/>
@@ -5361,7 +5468,7 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="4" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
       <c r="B12" s="15"/>
       <c r="D12" s="7"/>
@@ -5369,31 +5476,31 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="15" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
       <c r="B13" s="4"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
     </row>
     <row r="14" spans="1:5" ht="25.5">
       <c r="A14" s="15"/>
       <c r="B14" s="15" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="25"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="24"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="20"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="19"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="8"/>
@@ -5408,34 +5515,34 @@
       <c r="E18" s="7"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="20"/>
+      <c r="A19" s="19"/>
       <c r="B19" s="7"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="7"/>
@@ -9361,188 +9468,265 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B24" sqref="A1:B24"/>
+    <sheetView topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="39.7109375" customWidth="1"/>
-    <col min="2" max="2" width="28.85546875" customWidth="1"/>
+    <col min="1" max="1" width="39.7109375" style="39" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" style="39" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="35" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="36" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="15"/>
+      <c r="B3" s="36"/>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="15"/>
+      <c r="B4" s="36"/>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="36" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="34" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="18">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="22"/>
-    </row>
-    <row r="8" spans="1:2" ht="51">
-      <c r="A8" s="9" t="s">
-        <v>68</v>
+      <c r="B7" s="30"/>
+    </row>
+    <row r="8" spans="1:2" ht="18">
+      <c r="A8" s="33" t="s">
+        <v>148</v>
       </c>
-      <c r="B8" s="4"/>
-    </row>
-    <row r="9" spans="1:2" ht="38.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="9" t="s">
-        <v>69</v>
+      <c r="B8" s="21"/>
+    </row>
+    <row r="9" spans="1:2" ht="18">
+      <c r="A9" s="33" t="s">
+        <v>149</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="18">
-      <c r="A10" s="23" t="s">
+      <c r="B9" s="21"/>
+    </row>
+    <row r="10" spans="1:2" ht="28.5">
+      <c r="A10" s="33" t="s">
+        <v>150</v>
+      </c>
+      <c r="B10" s="21"/>
+    </row>
+    <row r="11" spans="1:2" ht="32.25" customHeight="1">
+      <c r="A11" s="37"/>
+      <c r="B11" s="38" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="18">
+      <c r="A12" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="23"/>
-    </row>
-    <row r="11" spans="1:2" ht="102">
-      <c r="A11" s="9" t="s">
+      <c r="B12" s="31"/>
+    </row>
+    <row r="13" spans="1:2" ht="18">
+      <c r="A13" s="33" t="s">
+        <v>148</v>
+      </c>
+      <c r="B13" s="22"/>
+    </row>
+    <row r="14" spans="1:2" ht="28.5">
+      <c r="A14" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="B14" s="22"/>
+    </row>
+    <row r="15" spans="1:2" ht="42.75">
+      <c r="A15" s="33" t="s">
+        <v>152</v>
+      </c>
+      <c r="B15" s="22"/>
+    </row>
+    <row r="16" spans="1:2" ht="28.5">
+      <c r="A16" s="33" t="s">
+        <v>153</v>
+      </c>
+      <c r="B16" s="22"/>
+    </row>
+    <row r="17" spans="1:2" ht="28.5">
+      <c r="A17" s="33"/>
+      <c r="B17" s="33" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="28.5">
+      <c r="A18" s="33"/>
+      <c r="B18" s="33" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="14.25">
+      <c r="A19" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="33"/>
+    </row>
+    <row r="20" spans="1:2" ht="14.25">
+      <c r="A20" s="33" t="s">
+        <v>148</v>
+      </c>
+      <c r="B20" s="33"/>
+    </row>
+    <row r="21" spans="1:2" ht="14.25">
+      <c r="A21" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="B21" s="33"/>
+    </row>
+    <row r="22" spans="1:2" ht="28.5">
+      <c r="A22" s="33" t="s">
+        <v>150</v>
+      </c>
+      <c r="B22" s="33"/>
+    </row>
+    <row r="23" spans="1:2" ht="42.75">
+      <c r="A23" s="33"/>
+      <c r="B23" s="33" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="28.5">
+      <c r="A24" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" s="33"/>
+    </row>
+    <row r="25" spans="1:2" ht="28.5">
+      <c r="A25" s="33"/>
+      <c r="B25" s="33" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="14.25">
+      <c r="A26" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="B11" s="10"/>
-    </row>
-    <row r="12" spans="1:2" ht="51">
-      <c r="A12" s="9"/>
-      <c r="B12" s="11" t="s">
-        <v>67</v>
+      <c r="B26" s="33"/>
+    </row>
+    <row r="27" spans="1:2" ht="42.75">
+      <c r="A27" s="33"/>
+      <c r="B27" s="33" t="s">
+        <v>156</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="18">
-      <c r="A13" s="23" t="s">
-        <v>24</v>
+    <row r="28" spans="1:2" ht="28.5">
+      <c r="A28" s="33"/>
+      <c r="B28" s="33" t="s">
+        <v>157</v>
       </c>
-      <c r="B13" s="23"/>
-    </row>
-    <row r="14" spans="1:2" ht="51">
-      <c r="A14" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="B14" s="11"/>
-    </row>
-    <row r="15" spans="1:2" ht="38.25">
-      <c r="A15" s="12"/>
-      <c r="B15" s="11" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="25.5">
-      <c r="A16" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="B16" s="11"/>
-    </row>
-    <row r="17" spans="1:2" ht="25.5">
-      <c r="A17" s="12"/>
-      <c r="B17" s="11" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="B18" s="11"/>
-    </row>
-    <row r="19" spans="1:2" ht="38.25">
-      <c r="A19" s="11"/>
-      <c r="B19" s="11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="18">
-      <c r="A20" s="23" t="s">
+    </row>
+    <row r="29" spans="1:2" ht="18">
+      <c r="A29" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="23"/>
-    </row>
-    <row r="21" spans="1:2" ht="51">
-      <c r="A21" s="11" t="s">
-        <v>68</v>
+      <c r="B29" s="31"/>
+    </row>
+    <row r="30" spans="1:2" ht="14.25">
+      <c r="A30" s="33" t="s">
+        <v>148</v>
       </c>
-      <c r="B21" s="10"/>
-    </row>
-    <row r="22" spans="1:2" ht="38.25">
-      <c r="A22" s="10"/>
-      <c r="B22" s="11" t="s">
-        <v>69</v>
+      <c r="B30" s="33"/>
+    </row>
+    <row r="31" spans="1:2" ht="14.25">
+      <c r="A31" s="33" t="s">
+        <v>149</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" ht="51">
-      <c r="A23" s="11" t="s">
-        <v>74</v>
+      <c r="B31" s="33"/>
+    </row>
+    <row r="32" spans="1:2" ht="28.5">
+      <c r="A32" s="33" t="s">
+        <v>150</v>
       </c>
-      <c r="B23" s="10"/>
-    </row>
-    <row r="24" spans="1:2" ht="38.25">
-      <c r="A24" s="10"/>
-      <c r="B24" s="11" t="s">
-        <v>75</v>
+      <c r="B32" s="33"/>
+    </row>
+    <row r="33" spans="1:2" ht="42.75">
+      <c r="A33" s="33"/>
+      <c r="B33" s="33" t="s">
+        <v>63</v>
       </c>
     </row>
+    <row r="34" spans="1:2" ht="28.5">
+      <c r="A34" s="33" t="s">
+        <v>158</v>
+      </c>
+      <c r="B34" s="33"/>
+    </row>
+    <row r="35" spans="1:2" ht="28.5">
+      <c r="A35" s="33" t="s">
+        <v>159</v>
+      </c>
+      <c r="B35" s="33"/>
+    </row>
+    <row r="36" spans="1:2" ht="28.5">
+      <c r="A36" s="33"/>
+      <c r="B36" s="33" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="28.5">
+      <c r="A37" s="33"/>
+      <c r="B37" s="33" t="s">
+        <v>161</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A29:B29"/>
   </mergeCells>
   <pageMargins left="0.51180555555555596" right="0.51180555555555596" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B44"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B32" sqref="A1:B32"/>
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="12.75"/>
@@ -9596,167 +9780,239 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="18">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="22"/>
-    </row>
-    <row r="8" spans="1:2" ht="38.25">
-      <c r="A8" s="9" t="s">
+      <c r="B7" s="30"/>
+    </row>
+    <row r="8" spans="1:2" ht="28.5">
+      <c r="A8" s="40" t="s">
+        <v>162</v>
+      </c>
+      <c r="B8" s="32"/>
+    </row>
+    <row r="9" spans="1:2" ht="28.5">
+      <c r="A9" s="40" t="s">
+        <v>163</v>
+      </c>
+      <c r="B9" s="32"/>
+    </row>
+    <row r="10" spans="1:2" ht="28.5">
+      <c r="A10" s="41"/>
+      <c r="B10" s="40" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="18">
+      <c r="A11" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="31"/>
+    </row>
+    <row r="12" spans="1:2" ht="28.5">
+      <c r="A12" s="40" t="s">
+        <v>162</v>
+      </c>
+      <c r="B12" s="40"/>
+    </row>
+    <row r="13" spans="1:2" ht="28.5">
+      <c r="A13" s="40" t="s">
+        <v>163</v>
+      </c>
+      <c r="B13" s="40"/>
+    </row>
+    <row r="14" spans="1:2" ht="28.5">
+      <c r="A14" s="40"/>
+      <c r="B14" s="40" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="28.5">
+      <c r="A15" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="B15" s="40"/>
+    </row>
+    <row r="16" spans="1:2" ht="42.75">
+      <c r="A16" s="40" t="s">
+        <v>165</v>
+      </c>
+      <c r="B16" s="40"/>
+    </row>
+    <row r="17" spans="1:2" ht="28.5">
+      <c r="A17" s="40" t="s">
+        <v>166</v>
+      </c>
+      <c r="B17" s="40"/>
+    </row>
+    <row r="18" spans="1:2" ht="14.25">
+      <c r="A18" s="40"/>
+      <c r="B18" s="40" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="28.5">
+      <c r="A19" s="40"/>
+      <c r="B19" s="40" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="18">
+      <c r="A20" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="31"/>
+    </row>
+    <row r="21" spans="1:2" ht="28.5">
+      <c r="A21" s="40" t="s">
+        <v>162</v>
+      </c>
+      <c r="B21" s="40"/>
+    </row>
+    <row r="22" spans="1:2" ht="28.5">
+      <c r="A22" s="40" t="s">
+        <v>169</v>
+      </c>
+      <c r="B22" s="40"/>
+    </row>
+    <row r="23" spans="1:2" ht="28.5">
+      <c r="A23" s="40"/>
+      <c r="B23" s="40" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="28.5">
+      <c r="A24" s="40" t="s">
+        <v>69</v>
+      </c>
+      <c r="B24" s="40"/>
+    </row>
+    <row r="25" spans="1:2" ht="28.5">
+      <c r="A25" s="40"/>
+      <c r="B25" s="40" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="14.25">
+      <c r="A26" s="40" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" s="40"/>
+    </row>
+    <row r="27" spans="1:2" ht="28.5">
+      <c r="A27" s="40"/>
+      <c r="B27" s="40" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="14.25">
+      <c r="A28" s="40" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" s="40"/>
+    </row>
+    <row r="29" spans="1:2" ht="14.25">
+      <c r="A29" s="40"/>
+      <c r="B29" s="40" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="28.5">
+      <c r="A30" s="40"/>
+      <c r="B30" s="40" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="18">
+      <c r="A31" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" s="31"/>
+    </row>
+    <row r="32" spans="1:2" ht="28.5">
+      <c r="A32" s="40" t="s">
+        <v>162</v>
+      </c>
+      <c r="B32" s="40"/>
+    </row>
+    <row r="33" spans="1:2" ht="28.5">
+      <c r="A33" s="40" t="s">
+        <v>163</v>
+      </c>
+      <c r="B33" s="40"/>
+    </row>
+    <row r="34" spans="1:2" ht="57">
+      <c r="A34" s="40" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" s="40"/>
+    </row>
+    <row r="35" spans="1:2" ht="28.5">
+      <c r="A35" s="40"/>
+      <c r="B35" s="40" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="28.5">
+      <c r="A36" s="40" t="s">
+        <v>69</v>
+      </c>
+      <c r="B36" s="40"/>
+    </row>
+    <row r="37" spans="1:2" ht="28.5">
+      <c r="A37" s="40"/>
+      <c r="B37" s="40" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="14.25">
+      <c r="A38" s="40" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" s="40"/>
+    </row>
+    <row r="39" spans="1:2" ht="28.5">
+      <c r="A39" s="40"/>
+      <c r="B39" s="40" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="14.25">
+      <c r="A40" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="B40" s="40"/>
+    </row>
+    <row r="41" spans="1:2" ht="28.5">
+      <c r="A41" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="B41" s="40"/>
+    </row>
+    <row r="42" spans="1:2" ht="42.75">
+      <c r="A42" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="4"/>
-    </row>
-    <row r="9" spans="1:2" ht="25.5">
-      <c r="A9" s="4"/>
-      <c r="B9" s="9" t="s">
-        <v>77</v>
+      <c r="B42" s="40"/>
+    </row>
+    <row r="43" spans="1:2" ht="14.25">
+      <c r="A43" s="40"/>
+      <c r="B43" s="40" t="s">
+        <v>175</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="18">
-      <c r="A10" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="23"/>
-    </row>
-    <row r="11" spans="1:2" ht="38.25">
-      <c r="A11" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="B11" s="10"/>
-    </row>
-    <row r="12" spans="1:2" ht="25.5">
-      <c r="A12" s="9"/>
-      <c r="B12" s="11" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="89.25">
-      <c r="A13" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="B13" s="10"/>
-    </row>
-    <row r="14" spans="1:2" ht="38.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="18">
-      <c r="A15" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="23"/>
-    </row>
-    <row r="16" spans="1:2" ht="38.25">
-      <c r="A16" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="B16" s="11"/>
-    </row>
-    <row r="17" spans="1:2" ht="25.5">
-      <c r="A17" s="12"/>
-      <c r="B17" s="11" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="25.5">
-      <c r="A18" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="B18" s="11"/>
-    </row>
-    <row r="19" spans="1:2" ht="25.5">
-      <c r="A19" s="12"/>
-      <c r="B19" s="11" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="B20" s="11"/>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="11"/>
-      <c r="B21" s="11" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="B22" s="11"/>
-    </row>
-    <row r="23" spans="1:2" ht="38.25">
-      <c r="A23" s="11"/>
-      <c r="B23" s="11" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="18">
-      <c r="A24" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="B24" s="23"/>
-    </row>
-    <row r="25" spans="1:2" ht="38.25">
-      <c r="A25" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="B25" s="10"/>
-    </row>
-    <row r="26" spans="1:2" ht="25.5">
-      <c r="A26" s="10"/>
-      <c r="B26" s="11" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="25.5">
-      <c r="A27" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="B27" s="10"/>
-    </row>
-    <row r="28" spans="1:2" ht="25.5">
-      <c r="A28" s="10"/>
-      <c r="B28" s="11" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B29" s="4"/>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="38.25">
-      <c r="A31" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="B31" s="4"/>
-    </row>
-    <row r="32" spans="1:2" ht="38.25">
-      <c r="A32" s="4"/>
-      <c r="B32" s="17" t="s">
-        <v>89</v>
+    <row r="44" spans="1:2" ht="28.5">
+      <c r="A44" s="40"/>
+      <c r="B44" s="40" t="s">
+        <v>174</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A31:B31"/>
   </mergeCells>
   <pageMargins left="0.51180555555555596" right="0.51180555555555596" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -9765,10 +10021,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B7" sqref="A1:B7"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="12.75"/>
@@ -9823,10 +10079,28 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="127.5">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2" t="s">
-        <v>49</v>
+    <row r="7" spans="1:2" ht="28.5">
+      <c r="A7" s="40"/>
+      <c r="B7" s="40" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="42.75">
+      <c r="A8" s="40"/>
+      <c r="B8" s="40" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="28.5">
+      <c r="A9" s="40"/>
+      <c r="B9" s="40" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="47.25" customHeight="1">
+      <c r="A10" s="40"/>
+      <c r="B10" s="40" t="s">
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -9837,10 +10111,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B14" sqref="A1:B14"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="12.75"/>
@@ -9854,7 +10128,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -9894,57 +10168,75 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="18">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="22"/>
-    </row>
-    <row r="8" spans="1:2" ht="51">
-      <c r="A8" s="9" t="s">
-        <v>90</v>
+      <c r="B7" s="30"/>
+    </row>
+    <row r="8" spans="1:2" ht="28.5">
+      <c r="A8" s="40" t="s">
+        <v>162</v>
       </c>
-      <c r="B8" s="4"/>
-    </row>
-    <row r="9" spans="1:2" ht="25.5">
-      <c r="A9" s="4"/>
-      <c r="B9" s="9" t="s">
-        <v>91</v>
+      <c r="B8" s="40"/>
+    </row>
+    <row r="9" spans="1:2" ht="28.5">
+      <c r="A9" s="40" t="s">
+        <v>180</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="18">
-      <c r="A10" s="23" t="s">
+      <c r="B9" s="40"/>
+    </row>
+    <row r="10" spans="1:2" ht="28.5">
+      <c r="A10" s="4"/>
+      <c r="B10" s="40" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="18">
+      <c r="A11" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="23"/>
-    </row>
-    <row r="11" spans="1:2" ht="51">
-      <c r="A11" s="11" t="s">
-        <v>90</v>
+      <c r="B11" s="31"/>
+    </row>
+    <row r="12" spans="1:2" ht="28.5">
+      <c r="A12" s="40" t="s">
+        <v>162</v>
       </c>
-      <c r="B11" s="10"/>
-    </row>
-    <row r="12" spans="1:2" ht="25.5">
-      <c r="A12" s="10"/>
-      <c r="B12" s="11" t="s">
-        <v>91</v>
+      <c r="B12" s="40"/>
+    </row>
+    <row r="13" spans="1:2" ht="28.5">
+      <c r="A13" s="40" t="s">
+        <v>180</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" ht="25.5">
-      <c r="A13" s="11" t="s">
-        <v>92</v>
+      <c r="B13" s="40"/>
+    </row>
+    <row r="14" spans="1:2" ht="28.5">
+      <c r="A14" s="40"/>
+      <c r="B14" s="40" t="s">
+        <v>77</v>
       </c>
-      <c r="B13" s="10"/>
-    </row>
-    <row r="14" spans="1:2" ht="38.25">
-      <c r="A14" s="10"/>
-      <c r="B14" s="11" t="s">
-        <v>93</v>
+    </row>
+    <row r="15" spans="1:2" ht="28.5">
+      <c r="A15" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="B15" s="40"/>
+    </row>
+    <row r="16" spans="1:2" ht="14.25">
+      <c r="A16" s="40"/>
+      <c r="B16" s="40" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="28.5">
+      <c r="A17" s="40"/>
+      <c r="B17" s="40" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
   </mergeCells>
   <pageMargins left="0.51180555555555596" right="0.51180555555555596" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -9953,10 +10245,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B12" sqref="A1:B12"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="12.75"/>
@@ -9970,7 +10262,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -10010,45 +10302,69 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="18">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="22"/>
-    </row>
-    <row r="8" spans="1:2" ht="51">
-      <c r="A8" s="9" t="s">
-        <v>94</v>
+      <c r="B7" s="30"/>
+    </row>
+    <row r="8" spans="1:2" ht="28.5">
+      <c r="A8" s="42" t="s">
+        <v>162</v>
       </c>
-      <c r="B8" s="4"/>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="4"/>
-      <c r="B9" s="9" t="s">
-        <v>95</v>
+      <c r="B8" s="42"/>
+    </row>
+    <row r="9" spans="1:2" ht="28.5">
+      <c r="A9" s="42" t="s">
+        <v>183</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="18">
-      <c r="A10" s="23" t="s">
+      <c r="B9" s="42"/>
+    </row>
+    <row r="10" spans="1:2" ht="14.25">
+      <c r="A10" s="42"/>
+      <c r="B10" s="42" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="18">
+      <c r="A11" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="23"/>
-    </row>
-    <row r="11" spans="1:2" ht="102">
-      <c r="A11" s="11" t="s">
-        <v>96</v>
+      <c r="B11" s="44"/>
+    </row>
+    <row r="12" spans="1:2" ht="28.5">
+      <c r="A12" s="42" t="s">
+        <v>162</v>
       </c>
-      <c r="B11" s="10"/>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="10"/>
-      <c r="B12" s="11" t="s">
-        <v>97</v>
+      <c r="B12" s="42"/>
+    </row>
+    <row r="13" spans="1:2" ht="28.5">
+      <c r="A13" s="42" t="s">
+        <v>183</v>
+      </c>
+      <c r="B13" s="42"/>
+    </row>
+    <row r="14" spans="1:2" ht="42.75">
+      <c r="A14" s="42" t="s">
+        <v>184</v>
+      </c>
+      <c r="B14" s="42"/>
+    </row>
+    <row r="15" spans="1:2" ht="42.75">
+      <c r="A15" s="42" t="s">
+        <v>185</v>
+      </c>
+      <c r="B15" s="42"/>
+    </row>
+    <row r="16" spans="1:2" ht="28.5">
+      <c r="A16" s="42"/>
+      <c r="B16" s="42" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
   </mergeCells>
   <pageMargins left="0.51180555555555596" right="0.51180555555555596" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -10057,10 +10373,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:B979"/>
+  <dimension ref="A1:B983"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B11" sqref="A1:B11"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="12.75"/>
@@ -10075,7 +10391,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -10093,11 +10409,11 @@
       <c r="B3" s="15"/>
     </row>
     <row r="4" spans="1:2" ht="76.5">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="34" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -10115,50 +10431,58 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="18">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="23"/>
-    </row>
-    <row r="8" spans="1:2" ht="76.5">
-      <c r="A8" s="11" t="s">
-        <v>101</v>
+      <c r="B7" s="31"/>
+    </row>
+    <row r="8" spans="1:2" ht="28.5">
+      <c r="A8" s="42" t="s">
+        <v>124</v>
       </c>
-      <c r="B8" s="10"/>
-    </row>
-    <row r="9" spans="1:2" ht="25.5">
-      <c r="A9" s="10"/>
-      <c r="B9" s="11" t="s">
-        <v>98</v>
+      <c r="B8" s="42"/>
+    </row>
+    <row r="9" spans="1:2" ht="28.5">
+      <c r="A9" s="42" t="s">
+        <v>186</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="51">
-      <c r="A10" s="11" t="s">
-        <v>99</v>
+      <c r="B9" s="42"/>
+    </row>
+    <row r="10" spans="1:2" ht="14.25">
+      <c r="A10" s="42" t="s">
+        <v>187</v>
       </c>
-      <c r="B10" s="10"/>
-    </row>
-    <row r="11" spans="1:2" ht="25.5">
-      <c r="A11" s="10"/>
-      <c r="B11" s="11" t="s">
-        <v>100</v>
+      <c r="B10" s="42"/>
+    </row>
+    <row r="11" spans="1:2" ht="14.25">
+      <c r="A11" s="42" t="s">
+        <v>188</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
+      <c r="B11" s="42"/>
+    </row>
+    <row r="12" spans="1:2" ht="28.5">
+      <c r="A12" s="42"/>
+      <c r="B12" s="42" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="28.5">
+      <c r="A13" s="42" t="s">
+        <v>189</v>
+      </c>
+      <c r="B13" s="42"/>
+    </row>
+    <row r="14" spans="1:2" ht="28.5">
+      <c r="A14" s="42" t="s">
+        <v>190</v>
+      </c>
+      <c r="B14" s="42"/>
+    </row>
+    <row r="15" spans="1:2" ht="28.5">
+      <c r="A15" s="42"/>
+      <c r="B15" s="42" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="8"/>
@@ -14015,6 +14339,22 @@
     <row r="979" spans="1:2">
       <c r="A979" s="8"/>
       <c r="B979" s="8"/>
+    </row>
+    <row r="980" spans="1:2">
+      <c r="A980" s="8"/>
+      <c r="B980" s="8"/>
+    </row>
+    <row r="981" spans="1:2">
+      <c r="A981" s="8"/>
+      <c r="B981" s="8"/>
+    </row>
+    <row r="982" spans="1:2">
+      <c r="A982" s="8"/>
+      <c r="B982" s="8"/>
+    </row>
+    <row r="983" spans="1:2">
+      <c r="A983" s="8"/>
+      <c r="B983" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -14030,7 +14370,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B9" sqref="A1:B9"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="12.75"/>
@@ -14044,7 +14384,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -14068,7 +14408,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -14087,20 +14427,20 @@
     </row>
     <row r="7" spans="1:2" ht="25.5">
       <c r="A7" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="3"/>
       <c r="B8" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="3"/>
       <c r="B9" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -14111,10 +14451,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B7" sqref="A1:B7"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="12.75"/>
@@ -14128,7 +14468,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -14136,7 +14476,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -14148,11 +14488,11 @@
       </c>
     </row>
     <row r="4" spans="1:2" ht="38.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="34" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -14169,11 +14509,17 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="51">
-      <c r="A7" s="2" t="s">
-        <v>62</v>
+    <row r="7" spans="1:2" ht="25.5">
+      <c r="A7" s="27" t="s">
+        <v>191</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="15"/>
+    </row>
+    <row r="8" spans="1:2" ht="25.5">
+      <c r="A8" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="B8" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.51180555555555596" right="0.51180555555555596" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
@@ -14183,10 +14529,10 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="12.75"/>
@@ -14195,15 +14541,15 @@
     <col min="2" max="2" width="44.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -14211,7 +14557,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -14219,21 +14565,21 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="51">
+    <row r="4" spans="1:2" ht="51">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -14241,14 +14587,17 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="38.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2" t="s">
-        <v>65</v>
+    <row r="7" spans="1:2" ht="25.5">
+      <c r="A7" s="15"/>
+      <c r="B7" s="15" t="s">
+        <v>193</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="D8" s="16"/>
+    <row r="8" spans="1:2">
+      <c r="A8" s="15"/>
+      <c r="B8" s="15" t="s">
+        <v>194</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.51180555555555596" right="0.51180555555555596" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
@@ -14320,7 +14669,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="B7" s="3"/>
     </row>
@@ -14332,14 +14681,14 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="4" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="B9" s="15"/>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -18360,38 +18709,38 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="15" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="B7" s="3"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="15"/>
       <c r="B8" s="3" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="4" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="B9" s="4"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="15"/>
       <c r="B10" s="15" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="25.5">
       <c r="A11" s="15"/>
       <c r="B11" s="15" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="15"/>
       <c r="B12" s="15" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -22398,62 +22747,62 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="17.850000000000001" customHeight="1">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="22"/>
+      <c r="B7" s="30"/>
     </row>
     <row r="8" spans="1:2" ht="17.850000000000001" customHeight="1">
-      <c r="A8" s="27" t="s">
-        <v>143</v>
+      <c r="A8" s="26" t="s">
+        <v>124</v>
       </c>
-      <c r="B8" s="18"/>
+      <c r="B8" s="17"/>
     </row>
     <row r="9" spans="1:2" ht="17.850000000000001" customHeight="1">
-      <c r="A9" s="27" t="s">
-        <v>145</v>
+      <c r="A9" s="26" t="s">
+        <v>126</v>
       </c>
-      <c r="B9" s="18"/>
+      <c r="B9" s="17"/>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="28" t="s">
-        <v>144</v>
+      <c r="A10" s="27" t="s">
+        <v>125</v>
       </c>
       <c r="B10" s="4"/>
     </row>
     <row r="11" spans="1:2" ht="25.5">
       <c r="A11" s="4"/>
-      <c r="B11" s="28" t="s">
-        <v>146</v>
+      <c r="B11" s="27" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="25.5">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="27" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="9"/>
     </row>
     <row r="13" spans="1:2" ht="17.850000000000001" customHeight="1">
-      <c r="A13" s="23" t="s">
+      <c r="A13" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="23"/>
+      <c r="B13" s="31"/>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="28" t="s">
-        <v>143</v>
+      <c r="A14" s="27" t="s">
+        <v>124</v>
       </c>
       <c r="B14" s="10"/>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="28" t="s">
-        <v>145</v>
+      <c r="A15" s="27" t="s">
+        <v>126</v>
       </c>
       <c r="B15" s="10"/>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="28" t="s">
-        <v>147</v>
+      <c r="A16" s="27" t="s">
+        <v>128</v>
       </c>
       <c r="B16" s="10"/>
     </row>
@@ -22464,14 +22813,14 @@
       </c>
     </row>
     <row r="18" spans="1:2" ht="25.5">
-      <c r="A18" s="28" t="s">
-        <v>149</v>
+      <c r="A18" s="27" t="s">
+        <v>130</v>
       </c>
       <c r="B18" s="11"/>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="28" t="s">
-        <v>148</v>
+      <c r="A19" s="27" t="s">
+        <v>129</v>
       </c>
       <c r="B19" s="10"/>
     </row>
@@ -22488,32 +22837,32 @@
       <c r="B21" s="10"/>
     </row>
     <row r="22" spans="1:2" ht="17.850000000000001" customHeight="1">
-      <c r="A22" s="23" t="s">
+      <c r="A22" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="23"/>
+      <c r="B22" s="31"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="29" t="s">
-        <v>143</v>
+      <c r="A23" s="28" t="s">
+        <v>124</v>
       </c>
       <c r="B23" s="11"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="29" t="s">
-        <v>145</v>
+      <c r="A24" s="28" t="s">
+        <v>126</v>
       </c>
       <c r="B24" s="11"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="29" t="s">
-        <v>151</v>
+      <c r="A25" s="28" t="s">
+        <v>132</v>
       </c>
       <c r="B25" s="11"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="29" t="s">
-        <v>150</v>
+      <c r="A26" s="28" t="s">
+        <v>131</v>
       </c>
       <c r="B26" s="11"/>
     </row>
@@ -22542,26 +22891,26 @@
       <c r="B30" s="11"/>
     </row>
     <row r="31" spans="1:2" ht="17.850000000000001" customHeight="1">
-      <c r="A31" s="23" t="s">
+      <c r="A31" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="B31" s="23"/>
+      <c r="B31" s="31"/>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="29" t="s">
-        <v>143</v>
+      <c r="A32" s="28" t="s">
+        <v>124</v>
       </c>
       <c r="B32" s="10"/>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="29" t="s">
-        <v>145</v>
+      <c r="A33" s="28" t="s">
+        <v>126</v>
       </c>
       <c r="B33" s="10"/>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="29" t="s">
-        <v>152</v>
+      <c r="A34" s="28" t="s">
+        <v>133</v>
       </c>
       <c r="B34" s="10"/>
     </row>
@@ -26641,153 +26990,153 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="18">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="22"/>
+      <c r="B7" s="30"/>
     </row>
     <row r="8" spans="1:2" ht="25.5">
-      <c r="A8" s="28" t="s">
-        <v>153</v>
+      <c r="A8" s="27" t="s">
+        <v>134</v>
       </c>
       <c r="B8" s="4"/>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="B9" s="4"/>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="27"/>
+      <c r="B10" s="29" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="27" t="s">
+        <v>136</v>
+      </c>
+      <c r="B11" s="4"/>
+    </row>
+    <row r="12" spans="1:2" ht="25.5">
+      <c r="A12" s="4"/>
+      <c r="B12" s="27" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="18">
+      <c r="A13" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="31"/>
+    </row>
+    <row r="14" spans="1:2" ht="25.5">
+      <c r="A14" s="27" t="s">
+        <v>134</v>
+      </c>
+      <c r="B14" s="10"/>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="B15" s="10"/>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="27"/>
+      <c r="B16" s="28" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="B17" s="10"/>
+    </row>
+    <row r="18" spans="1:2" ht="25.5">
+      <c r="A18" s="9"/>
+      <c r="B18" s="28" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="25.5">
+      <c r="A19" s="9"/>
+      <c r="B19" s="28" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="25.5">
+      <c r="A20" s="27" t="s">
+        <v>141</v>
+      </c>
+      <c r="B20" s="10"/>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="9"/>
+      <c r="B21" s="28" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="18">
+      <c r="A22" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="31"/>
+    </row>
+    <row r="23" spans="1:2" ht="25.5">
+      <c r="A23" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="B23" s="11"/>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="B24" s="11"/>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="28"/>
+      <c r="B25" s="28" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="B26" s="11"/>
+    </row>
+    <row r="27" spans="1:2" ht="25.5">
+      <c r="A27" s="28"/>
+      <c r="B27" s="28" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="25.5">
+      <c r="A28" s="28" t="s">
         <v>145</v>
       </c>
-      <c r="B9" s="4"/>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="28"/>
-      <c r="B10" s="30" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="28" t="s">
-        <v>155</v>
-      </c>
-      <c r="B11" s="4"/>
-    </row>
-    <row r="12" spans="1:2" ht="25.5">
-      <c r="A12" s="4"/>
-      <c r="B12" s="28" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="18">
-      <c r="A13" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="23"/>
-    </row>
-    <row r="14" spans="1:2" ht="25.5">
-      <c r="A14" s="28" t="s">
-        <v>153</v>
-      </c>
-      <c r="B14" s="10"/>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="28" t="s">
-        <v>145</v>
-      </c>
-      <c r="B15" s="10"/>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="28"/>
-      <c r="B16" s="29" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="28" t="s">
-        <v>157</v>
-      </c>
-      <c r="B17" s="10"/>
-    </row>
-    <row r="18" spans="1:2" ht="25.5">
-      <c r="A18" s="9"/>
-      <c r="B18" s="29" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="25.5">
-      <c r="A19" s="9"/>
-      <c r="B19" s="29" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="25.5">
-      <c r="A20" s="28" t="s">
-        <v>160</v>
-      </c>
-      <c r="B20" s="10"/>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="9"/>
-      <c r="B21" s="29" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="18">
-      <c r="A22" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22" s="23"/>
-    </row>
-    <row r="23" spans="1:2" ht="25.5">
-      <c r="A23" s="29" t="s">
-        <v>153</v>
-      </c>
-      <c r="B23" s="11"/>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="29" t="s">
-        <v>145</v>
-      </c>
-      <c r="B24" s="11"/>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="29"/>
-      <c r="B25" s="29" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="29" t="s">
-        <v>162</v>
-      </c>
-      <c r="B26" s="11"/>
-    </row>
-    <row r="27" spans="1:2" ht="25.5">
-      <c r="A27" s="29"/>
-      <c r="B27" s="29" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="25.5">
-      <c r="A28" s="29" t="s">
-        <v>164</v>
-      </c>
       <c r="B28" s="11"/>
     </row>
     <row r="29" spans="1:2" ht="25.5">
       <c r="A29" s="12"/>
-      <c r="B29" s="29" t="s">
+      <c r="B29" s="28" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="25.5">
-      <c r="A30" s="29" t="s">
-        <v>165</v>
+      <c r="A30" s="28" t="s">
+        <v>146</v>
       </c>
       <c r="B30" s="11"/>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="12"/>
-      <c r="B31" s="29" t="s">
-        <v>166</v>
+      <c r="B31" s="28" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -30754,56 +31103,56 @@
     </row>
     <row r="7" spans="1:2" ht="25.5">
       <c r="A7" s="15" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="B7" s="3"/>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="4"/>
       <c r="B8" s="15" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="25.5">
       <c r="A9" s="15" t="s">
-        <v>118</v>
+        <v>99</v>
       </c>
       <c r="B9" s="15"/>
     </row>
     <row r="10" spans="1:2" ht="25.5">
       <c r="A10" s="15"/>
       <c r="B10" s="15" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="15" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="B11" s="15"/>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="4"/>
       <c r="B12" s="4" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="15" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="B13" s="15"/>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="15"/>
       <c r="B14" s="15" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="15"/>
       <c r="B15" s="15" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -34813,56 +35162,56 @@
     </row>
     <row r="7" spans="1:2" ht="25.5">
       <c r="A7" s="15" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="B7" s="3"/>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="4"/>
       <c r="B8" s="15" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="25.5">
       <c r="A9" s="15" t="s">
-        <v>120</v>
+        <v>101</v>
       </c>
       <c r="B9" s="15"/>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="15"/>
       <c r="B10" s="15" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="15" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
       <c r="B11" s="4"/>
     </row>
     <row r="12" spans="1:2" ht="25.5">
       <c r="A12" s="4"/>
       <c r="B12" s="15" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="15" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="B13" s="15"/>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="4"/>
       <c r="B14" s="15" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="25.5">
       <c r="A15" s="15"/>
       <c r="B15" s="15" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -38881,117 +39230,117 @@
     </row>
     <row r="7" spans="1:7" ht="25.5">
       <c r="A7" s="15" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="B7" s="3"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4"/>
       <c r="B8" s="15" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
-      <c r="D8" s="20"/>
+      <c r="D8" s="19"/>
       <c r="E8" s="7"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="19"/>
     </row>
     <row r="9" spans="1:7" ht="25.5">
       <c r="A9" s="15" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
       <c r="B9" s="15"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
       <c r="F9" s="7"/>
-      <c r="G9" s="20"/>
+      <c r="G9" s="19"/>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="15"/>
       <c r="B10" s="15" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
       <c r="F10" s="7"/>
-      <c r="G10" s="20"/>
+      <c r="G10" s="19"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="15" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="B11" s="4"/>
-      <c r="D11" s="20"/>
+      <c r="D11" s="19"/>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
-      <c r="G11" s="20"/>
+      <c r="G11" s="19"/>
     </row>
     <row r="12" spans="1:7" ht="25.5">
       <c r="A12" s="4"/>
       <c r="B12" s="15" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
-      <c r="D12" s="20"/>
+      <c r="D12" s="19"/>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
-      <c r="G12" s="20"/>
+      <c r="G12" s="19"/>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="15" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="B13" s="4"/>
-      <c r="D13" s="20"/>
+      <c r="D13" s="19"/>
       <c r="E13" s="7"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="15"/>
       <c r="B14" s="15" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
       <c r="F14" s="7"/>
-      <c r="G14" s="20"/>
+      <c r="G14" s="19"/>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="15"/>
       <c r="B15" s="15" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
-      <c r="D15" s="20"/>
+      <c r="D15" s="19"/>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
-      <c r="G15" s="20"/>
+      <c r="G15" s="19"/>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
       <c r="F16" s="7"/>
-      <c r="G16" s="20"/>
+      <c r="G16" s="19"/>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
-      <c r="D17" s="20"/>
+      <c r="D17" s="19"/>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
-      <c r="G17" s="20"/>
+      <c r="G17" s="19"/>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="8"/>
@@ -42988,56 +43337,56 @@
     </row>
     <row r="7" spans="1:2" ht="25.5">
       <c r="A7" s="15" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="B7" s="3"/>
     </row>
     <row r="8" spans="1:2" ht="38.25">
       <c r="A8" s="15"/>
       <c r="B8" s="15" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="25.5">
+    <row r="9" spans="1:2">
       <c r="A9" s="15"/>
       <c r="B9" s="15" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="4" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
       <c r="B10" s="4"/>
     </row>
     <row r="11" spans="1:2" ht="25.5">
       <c r="A11" s="4"/>
-      <c r="B11" s="17" t="s">
-        <v>139</v>
+      <c r="B11" s="16" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="4" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
       <c r="B12" s="4"/>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="24" t="s">
-        <v>137</v>
+      <c r="A13" s="23" t="s">
+        <v>118</v>
       </c>
       <c r="B13" s="4"/>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="15" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
       <c r="B14" s="15"/>
     </row>
     <row r="15" spans="1:2" ht="25.5">
       <c r="A15" s="15"/>
       <c r="B15" s="15" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:2">

</xml_diff>